<commit_message>
[ADD] module acm, alb, route53
</commit_message>
<xml_diff>
--- a/Activity TEDS ASP.xlsx
+++ b/Activity TEDS ASP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tunasgroup-my.sharepoint.com/personal/muhammad_bella_tunasgroup_com/Documents/SysAdmin Dokumentasi/Migrate AWS TUNAS GROUP/AWS/TDM/Migrate 2023/ASP/TEDS ASP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bellabeen/development/terraform/terrraform-odoo-aws/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="11_0A208F665366638C9249BFBC9C3F7AA88AD6D195" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9DBF848-8709-2C41-A539-C2A420E61746}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131B9BBB-EBC5-C94A-AF3F-ADA820A42F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="143">
   <si>
     <t>No</t>
   </si>
@@ -476,12 +476,19 @@
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="dd\-mmm\-yyyy\ hh:mm"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -686,14 +693,14 @@
   </cellStyleXfs>
   <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -718,7 +725,7 @@
     <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -740,57 +747,57 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1071,7 +1078,7 @@
   <dimension ref="B3:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1081,26 +1088,26 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="39" t="s">
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="40" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="22">
         <v>1</v>
       </c>
@@ -1116,13 +1123,13 @@
       <c r="H4" s="22">
         <v>5</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="40"/>
     </row>
     <row r="5" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="23"/>
       <c r="E5" s="28"/>
       <c r="F5" s="28"/>
@@ -1136,7 +1143,7 @@
       <c r="B6" s="24">
         <v>2</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="35" t="s">
         <v>139</v>
       </c>
       <c r="D6" s="23"/>
@@ -1152,7 +1159,7 @@
       <c r="B7" s="24">
         <v>3</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="35" t="s">
         <v>140</v>
       </c>
       <c r="D7" s="23"/>
@@ -1168,7 +1175,7 @@
       <c r="B8" s="24">
         <v>4</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="35" t="s">
         <v>141</v>
       </c>
       <c r="D8" s="23"/>
@@ -1184,7 +1191,7 @@
       <c r="B9" s="24">
         <v>5</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="35" t="s">
         <v>142</v>
       </c>
       <c r="D9" s="23"/>
@@ -1222,7 +1229,7 @@
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
-      <c r="I11" s="31"/>
+      <c r="I11" s="43"/>
     </row>
     <row r="12" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="24">
@@ -1279,7 +1286,7 @@
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
       <c r="I15" s="43" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="16" x14ac:dyDescent="0.2">
@@ -1294,7 +1301,9 @@
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
-      <c r="I16" s="31"/>
+      <c r="I16" s="43" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="24">
@@ -1339,10 +1348,10 @@
       <c r="I19" s="31"/>
     </row>
     <row r="20" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="36"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="23"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
@@ -1491,10 +1500,10 @@
       <c r="I30" s="31"/>
     </row>
     <row r="31" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="36"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
       <c r="F31" s="28"/>
@@ -1531,10 +1540,10 @@
       <c r="I33" s="31"/>
     </row>
     <row r="34" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="36"/>
+      <c r="C34" s="37"/>
       <c r="D34" s="28"/>
       <c r="E34" s="28"/>
       <c r="F34" s="28"/>
@@ -1557,10 +1566,10 @@
       <c r="I35" s="31"/>
     </row>
     <row r="36" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="36"/>
+      <c r="C36" s="37"/>
       <c r="D36" s="28"/>
       <c r="E36" s="28"/>
       <c r="F36" s="28"/>
@@ -2135,18 +2144,18 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="41" t="s">
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
     </row>
     <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">

</xml_diff>

<commit_message>
[FIX] module asg for launch template and autoscalling
</commit_message>
<xml_diff>
--- a/Activity TEDS ASP.xlsx
+++ b/Activity TEDS ASP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bellabeen/development/terraform/terrraform-odoo-aws/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C92CBE-079C-E541-92A7-0A9DB41CC1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C852C6-E5F3-774D-AE8E-41713A04BEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="145">
   <si>
     <t>No</t>
   </si>
@@ -482,12 +482,19 @@
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="dd\-mmm\-yyyy\ hh:mm"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -711,16 +718,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -745,7 +752,7 @@
     <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -767,58 +774,59 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1100,7 +1108,7 @@
   <dimension ref="B3:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1110,26 +1118,26 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="42" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="43" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="22">
         <v>1</v>
       </c>
@@ -1145,13 +1153,13 @@
       <c r="H4" s="22">
         <v>5</v>
       </c>
-      <c r="I4" s="42"/>
+      <c r="I4" s="43"/>
     </row>
     <row r="5" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="39"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="23"/>
       <c r="E5" s="28"/>
       <c r="F5" s="28"/>
@@ -1237,7 +1245,7 @@
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
-      <c r="I10" s="45" t="s">
+      <c r="I10" s="38" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1301,7 +1309,7 @@
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
-      <c r="I14" s="45" t="s">
+      <c r="I14" s="38" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1333,7 +1341,7 @@
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
-      <c r="I16" s="45" t="s">
+      <c r="I16" s="38" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1349,7 +1357,7 @@
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
-      <c r="I17" s="45" t="s">
+      <c r="I17" s="38" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1365,7 +1373,7 @@
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
       <c r="H18" s="28"/>
-      <c r="I18" s="45" t="s">
+      <c r="I18" s="38" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1379,7 +1387,9 @@
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
-      <c r="I19" s="45"/>
+      <c r="I19" s="46" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="24">
@@ -1393,15 +1403,15 @@
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
-      <c r="I20" s="45" t="s">
+      <c r="I20" s="38" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="39"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="23"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
@@ -1550,10 +1560,10 @@
       <c r="I31" s="31"/>
     </row>
     <row r="32" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="39"/>
+      <c r="C32" s="40"/>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
@@ -1590,10 +1600,10 @@
       <c r="I34" s="31"/>
     </row>
     <row r="35" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B35" s="38" t="s">
+      <c r="B35" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="39"/>
+      <c r="C35" s="40"/>
       <c r="D35" s="28"/>
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
@@ -1616,10 +1626,10 @@
       <c r="I36" s="31"/>
     </row>
     <row r="37" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="39"/>
+      <c r="C37" s="40"/>
       <c r="D37" s="28"/>
       <c r="E37" s="28"/>
       <c r="F37" s="28"/>
@@ -2194,18 +2204,18 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="44" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
     </row>
     <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">

</xml_diff>